<commit_message>
INCLUSÃO DE NOVAS ABAS
> SOMASE
>SOMASES
>SUBTOTAL
>SOMAXMY2
</commit_message>
<xml_diff>
--- a/simples/SOMAS.xlsx
+++ b/simples/SOMAS.xlsx
@@ -1,41 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zoooo\Documents\GitHub\excel\simples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04B3A583-0259-47B0-A389-E4174AA480B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0A2C7F-B8AB-4392-B314-9FF22E480D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{06E2FBEE-D8D8-47C0-8849-A6FB9C5F4F1B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{06E2FBEE-D8D8-47C0-8849-A6FB9C5F4F1B}"/>
   </bookViews>
   <sheets>
     <sheet name="SOMA COMUM" sheetId="1" r:id="rId1"/>
     <sheet name="SOMA DOS QUADRADOS" sheetId="3" r:id="rId2"/>
     <sheet name="SOMAR PRODUTO" sheetId="4" r:id="rId3"/>
+    <sheet name="SOMASE&amp;SOMASES" sheetId="5" r:id="rId4"/>
+    <sheet name="SUBTOTAL" sheetId="6" r:id="rId5"/>
+    <sheet name="SOMAXMY2" sheetId="8" r:id="rId6"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">SUBTOTAL!$A$1:$C$9</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
   <si>
     <t>Aluno</t>
   </si>
@@ -137,6 +135,90 @@
   </si>
   <si>
     <t>SOMA PRODUTO APENAS DOS ITENS C E A:</t>
+  </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Preço</t>
+  </si>
+  <si>
+    <t>k2</t>
+  </si>
+  <si>
+    <t>k3</t>
+  </si>
+  <si>
+    <t>Qtd total</t>
+  </si>
+  <si>
+    <t>Soma de um item sem levar em conta a posição</t>
+  </si>
+  <si>
+    <t>Qtd</t>
+  </si>
+  <si>
+    <t>Soma dos itens levando em conta a posição</t>
+  </si>
+  <si>
+    <t>Posição</t>
+  </si>
+  <si>
+    <t>USO DA SOMA SES</t>
+  </si>
+  <si>
+    <t>USO DA SOMA SE</t>
+  </si>
+  <si>
+    <t>FUNCIONÁRIO</t>
+  </si>
+  <si>
+    <t>DESEMPENHO</t>
+  </si>
+  <si>
+    <t>joão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lucas </t>
+  </si>
+  <si>
+    <t>josé</t>
+  </si>
+  <si>
+    <t>maria</t>
+  </si>
+  <si>
+    <t>juca</t>
+  </si>
+  <si>
+    <t>mario</t>
+  </si>
+  <si>
+    <t>joana</t>
+  </si>
+  <si>
+    <t>michel</t>
+  </si>
+  <si>
+    <t>EQUIPE</t>
+  </si>
+  <si>
+    <t>DESEMPENHO TOTAL</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z = x - y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> z^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;---- Usando a função SOMA XMY2</t>
   </si>
 </sst>
 </file>
@@ -144,9 +226,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,8 +248,23 @@
       <name val="Cascadia Mono SemiBold"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,8 +283,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -195,11 +328,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,19 +456,77 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -261,7 +547,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -849,7 +1135,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -931,8 +1217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1A9B968-5B66-40B3-B34F-4C05CEF86123}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1093,4 +1379,570 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99495FF2-4DEB-4189-B008-E40C1669B6D1}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="18.90625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="20">
+        <v>56</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="22">
+        <v>12</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="22">
+        <v>5</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="22">
+        <v>2.5</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="22">
+        <v>2.5</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="25">
+        <v>80</v>
+      </c>
+      <c r="C7" s="26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+    </row>
+    <row r="10" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="29">
+        <f>SUMIF(A2:A7,B11,B2:B7)</f>
+        <v>73</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="29">
+        <f>SUMIFS(B2:B7,A2:A7,B16,C2:C7,B17)</f>
+        <v>68</v>
+      </c>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:E17"/>
+    <mergeCell ref="C9:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A016C133-4386-4C0B-819D-CFEC865BFF7D}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:T39"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="24.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.6328125" style="2" customWidth="1"/>
+    <col min="3" max="8" width="20.6328125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="35.6328125" style="34" customWidth="1"/>
+    <col min="10" max="10" width="26" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
+      <c r="T1" s="33"/>
+    </row>
+    <row r="2" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+    </row>
+    <row r="3" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33"/>
+      <c r="R3" s="33"/>
+      <c r="S3" s="33"/>
+      <c r="T3" s="33"/>
+    </row>
+    <row r="4" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+    </row>
+    <row r="15" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+    </row>
+    <row r="16" spans="1:20" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="36">
+        <f>SUBTOTAL(9, B2:B9)</f>
+        <v>16</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+    </row>
+    <row r="17" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <autoFilter ref="A1:C9" xr:uid="{A016C133-4386-4C0B-819D-CFEC865BFF7D}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="B"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124C809F-8577-4863-9336-94524E89A8D1}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="4" width="10.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <f>A2-B2</f>
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <f>C2*C2</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f>SUMXMY2(A2,B2)</f>
+        <v>36</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>